<commit_message>
food list in assets
</commit_message>
<xml_diff>
--- a/app/src/main/assets/basicfood.xlsx
+++ b/app/src/main/assets/basicfood.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakaddour\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakaddour\Documents\GitHub\InsuBete_ML\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,17 +15,11 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Glycemic Index</t>
   </si>
@@ -264,34 +258,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma0" xfId="3"/>
+    <cellStyle name="Comma0" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Book2" xfId="1"/>
-    <cellStyle name="Normal_International_GL_tables_2002 2" xfId="2"/>
+    <cellStyle name="Normal_Book2" xfId="2"/>
+    <cellStyle name="Normal_International_GL_tables_2002 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -569,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1241,216 +1235,211 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>150</v>
+      </c>
+      <c r="D48">
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C49">
         <v>150</v>
       </c>
       <c r="D49">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C50">
         <v>150</v>
       </c>
       <c r="D50">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C51">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C52">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="D52">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C53">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="D53">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C54">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D54">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C55">
-        <v>57</v>
+        <v>250</v>
       </c>
       <c r="D55">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C56">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D56">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C57">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C58">
-        <v>250</v>
+        <v>95</v>
       </c>
       <c r="D58">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C59">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="D59">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B60">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C60">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D60">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B61">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C61">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D61">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C62">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D62">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>66</v>
-      </c>
-      <c r="C63">
-        <v>80</v>
-      </c>
-      <c r="D63">
         <v>26</v>
       </c>
     </row>

</xml_diff>